<commit_message>
feat : end is final!
</commit_message>
<xml_diff>
--- a/UnityGPTapi.xlsx
+++ b/UnityGPTapi.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitThings\Wonder\2024-Spring-Capstone-team20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837FCBAF-8552-4E39-91FF-657C3B0B48DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C098F4-C6A6-4173-8A2B-AFC55D426797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{25586EBA-5156-4FCA-BD68-1ABD9FE0A969}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{25586EBA-5156-4FCA-BD68-1ABD9FE0A969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>unity init data</t>
   </si>
@@ -90,6 +91,147 @@
   </si>
   <si>
     <t>data: {'Request': '\n @ObjID =2, @ObjName = Cup, @ObjectInfo = blah, @defaultPrice =10, @expensvie = 100, @tooExpensive =200 \n @NpcID = 1, @NpcSex = female, @NpcAge = 17, @NpcPersonality = Bad, @NpcProplemType = relate, @NpcProblemInfo = blah', 'SendType': 'Init'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unity npcinit data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+        "Request": "\nName: 현민삐, Age: 24, Sex: Female\nSituation_Description: 아빠가 최근에 회사를 그만두셨고, 그 이후로 집안 경제가 어려워졌어. 네가 할 수 있는 게 많지 않아서 무력감을 느끼고 있어. 게다가 너도 졸업을 앞두고 진로에 대한 고민이 많아.\nPersonality: 너는 독립적이면서도 깊이 공감하는 성격을 가지고 있어. 가족에 대한 책임감을 자주 느끼고, 그 때문에 무언가 잘못되면 부담감을 느껴. 스스로 해결책을 찾기를 선호하지만, 가족의 문제로 인해 너의 결정을 올바르게 내릴 수 있을지 자주 의심해. 낯선 사람에게는 특히 스트레스가 많은 상황에서 신중하게 대하지만, 진심 어린 소통을 좋아해. 초면에 말을 거는 상인이 싫지는 않고, 대화를 즐기며 흥미를 느껴.\nDialogue_Style: 기본적으로 정중한 존댓말을 사용하지만 불쾌하거나 위협을 받으면 반말을 사용해. 현재 집안에 돈이 없기 때문에 너는 많은 돈을 쓰고 싶지 않아. 물건의 질보다 가격에 집중하는 편이고, 만약 물건이 너무 비싸다면 넌 물건 사기를 포기할거야. 넌 말이 많고 솔직해서 하고 싶은 말이 있으면 바로바로 하는 편이야.",
+        "SendType": "NpcInit"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "@ Npc Attached."
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpt npcinit data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unity chatsale data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpt chatsale data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unity iteminit data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpt iteminit data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "@ Item Attached."
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unity chatbargain data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Request": "$start", "SendType": "ChatBargain"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpt chatbargain data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "```json\n{\n  \"output\": {\n    \"decision\": \"wait\",\n    \"yourReply\": \"안녕하세요! 오늘 기분이 어떠신가요?\"\n  }\n}\n```"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "```json\n{\n  \"output\": {\n    \"decision\": \"yes\",\n    \"ThingToBuy\": \"핸드폰 케이스\",\n    \"yourReply\": \"이 핸드폰 케이스가 마음에 들어요! 사겠습니다.\",\n    \"summary\": \"이 핸드폰 케이스는 디자인이 마음에 들고, 가격도 적당해 보여서 구매하기로 결정했어요. 상인도 친절하게 대화해 주셔서 좋았어요.\"\n  }\n}\n```"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+        "Request": "지금 테스트 중인데 혹시 decision : no 예시 좀 줄 수 있어?",
+        "SendType": "ChatSale"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "```json\n{\n  \"output\": {\n    \"decision\": \"no\",\n    \"yourReply\": \"죄송하지만, 지금은 구매할 생각이 없어요.\",\n    \"summary\": \"상인은 친절했지만, 현재 집안 경제가 어려워서 물건을 사는 것이 부담스러웠어요. 대화는 즐거웠지만, 구매는 하지 않기로 결정했어요.\"\n  }\n}\n```"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "{\n  \"reaction\": \"이 책이 왜 이렇게 비싼지 궁금한데요. 동기부여 관련 책이긴 한데, 200 크레딧은 너무 비싼 것 같아요.\",\n  \"vendorSuggest\": 200,\n  \"yourSuggest\": 50,\n  \"persuasion\": -3\n}"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Request": "그래, 시원하게 깎을게! 100!", "SendType": "ChatBargain"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "{\n  \"reaction\": \"100 크레딧으로 줄 수 있다니, 그래도 200 크레딧보다는 나은 것 같아요. 하지만 이 책이 정말 동기부여에 도움이 될지 좀 더 설명해줄 수 있나요? 가격이 이렇게 비싼 이유가 궁금해요.\",\n  \"vendorSuggest\": 200,\n  \"yourSuggest\": 100,\n  \"persuasion\": -1\n}"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unity endpoint data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Request": "$buy", "SendType": "EndPoint"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Request": "$reject", "SendType": "EndPoint"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Request": "$leave", "SendType": "EndPoint"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpt endpoint data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+        "Request": "\nThe thing you want to buy: 동기부여 관련 책\nThe thing vendor is selling to you: 책\nvendor First Suggest: 200 credit,Your First Suggest: 50 credit yourOpinion: too expensive",
+        "SendType": "ItemInit"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "{\n  \"reaction\": \"저는 이 책을 사겠습니다. 가격이 너무 비쌌지만, 내용을 알고 싶어서요.\",\n  \"summary\": \"상인과의 대화에서 가격이 비싸다고 느꼈지만, 책의 내용을 알고 싶어서 결국 구매하기로 결정했습니다.\"\n}"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "{\n  \"reaction\": \"죄송하지만, 이 가격은 저에게 너무 비쌉니다. 다른 곳에서 더 나은 가격을 찾을 수 있을 것 같아요. 안녕히 계세요.\",\n  \"summary\": \"상인의 가격이 너무 비쌌고, 제시된 설명이 설득력이 없어서 구매를 포기하게 되었습니다. 상인의 태도는 그리 친절하지 않았고, 대화가 불편하게 느껴졌습니다.\"\n}"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "reply": "{\n  \"reaction\": \"이런, 더 이상 대화하고 싶지 않네요. 가격이 너무 비싸고 설명도 그다지 설득력이 없었어요. 그냥 떠나겠습니다.\",\n  \"summary\": \"상인이 제시한 가격이 너무 비쌌고, 그에 대한 설명이 부족했어요. 대화가 불편해져서 더 이상 이야기하고 싶지 않았습니다.\"\n}"
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -142,11 +284,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,7 +631,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6499DAD8-6ABB-4F19-9291-87C8910A78D5}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -496,86 +644,250 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>2</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F98C65F-8CC5-4724-8819-196A369A9AB9}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A22" sqref="A1:XFD22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+    <row r="11" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+    <row r="12" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+    <row r="13" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+    <row r="14" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+    <row r="15" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
+    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
deploy : another app
</commit_message>
<xml_diff>
--- a/UnityGPTapi.xlsx
+++ b/UnityGPTapi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitThings\Wonder\2024-Spring-Capstone-team20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C098F4-C6A6-4173-8A2B-AFC55D426797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C82F7C2-C8A1-4A98-B61F-57A11AD1C8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{25586EBA-5156-4FCA-BD68-1ABD9FE0A969}"/>
+    <workbookView xWindow="0" yWindow="1992" windowWidth="17280" windowHeight="8964" xr2:uid="{25586EBA-5156-4FCA-BD68-1ABD9FE0A969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,7 +284,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -293,9 +293,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6499DAD8-6ABB-4F19-9291-87C8910A78D5}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -801,93 +798,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>